<commit_message>
Sprint 2 Retrospective and Sprint 3 Backlogs
</commit_message>
<xml_diff>
--- a/SCRUM Files/Sprint 2 Backlog.xlsx
+++ b/SCRUM Files/Sprint 2 Backlog.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24426"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\csce315\CSCE-315-Project2-local\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Project 2 Group 4</t>
   </si>
@@ -66,6 +68,9 @@
     <t>Create Objects for 6 houses and 2 Kalah</t>
   </si>
   <si>
+    <t>Input 4 seeds in each house</t>
+  </si>
+  <si>
     <t>Take in user input by keyboard</t>
   </si>
   <si>
@@ -202,45 +207,16 @@
   </si>
   <si>
     <t>Andrew Lam/Tony Huynh</t>
-  </si>
-  <si>
-    <t>Input seeds in each house</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,20 +239,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -335,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -387,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -581,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,25 +562,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="53.5" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="3" max="3" width="53.53125" customWidth="1"/>
+    <col min="4" max="4" width="22.06640625" customWidth="1"/>
+    <col min="5" max="5" width="28.46484375" customWidth="1"/>
+    <col min="6" max="6" width="23.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -629,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -637,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>1.1000000000000001</v>
       </c>
@@ -648,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1.2</v>
       </c>
@@ -659,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1.3</v>
       </c>
@@ -669,199 +640,145 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>1.4</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>1.5</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>1.6</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>1.7</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>1.8</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>1.9</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>1.1100000000000001</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>1.1200000000000001</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>1.1299999999999999</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>1.1399999999999999</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>1.1499999999999999</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>1.1599999999999999</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -869,16 +786,16 @@
       <c r="E20" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>1.17</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -886,35 +803,35 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>2.1</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>2.2000000000000002</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -922,13 +839,16 @@
       <c r="E25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>2.2999999999999998</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -936,55 +856,67 @@
       <c r="E26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>2.4</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="F27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>2.5</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>2.6</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>2.7</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -992,13 +924,16 @@
       <c r="E30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>2.8</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1006,13 +941,16 @@
       <c r="E31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>2.9</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1020,43 +958,46 @@
       <c r="E32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B33" s="2">
         <v>2.1</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>2.11</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>3.1</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -1064,16 +1005,16 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>3.2</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1081,27 +1022,27 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>3.3</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>3.4</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1109,27 +1050,27 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>3.5</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>3.6</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -1137,16 +1078,16 @@
       <c r="E42" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>3.7</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1154,16 +1095,16 @@
       <c r="E43" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>3.8</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1171,117 +1112,120 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>4.0999999999999996</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>4.2</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>4.3</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>4.3</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>4.4000000000000004</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>4.5</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>4.5999999999999996</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>4.7</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>4.8</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D57">
         <f>SUM(D5:D19,D24:D34,D37:D44,D47:D54)</f>
@@ -1290,11 +1234,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>